<commit_message>
updating why miss file
</commit_message>
<xml_diff>
--- a/learn_bot/learn_bot/latent/vis/why_mis_filter_28.xlsx
+++ b/learn_bot/learn_bot/latent/vis/why_mis_filter_28.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -86,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -107,6 +108,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,16 +215,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -237,27 +247,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,7 +275,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,12 +287,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Pivot Table Corner" xfId="20"/>
-    <cellStyle name="Pivot Table Value" xfId="21"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
+    <cellStyle name="Pivot Table Corner" xfId="21"/>
     <cellStyle name="Pivot Table Field" xfId="22"/>
-    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Result" xfId="23"/>
     <cellStyle name="Pivot Table Title" xfId="24"/>
-    <cellStyle name="Pivot Table Result" xfId="25"/>
+    <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -593,106 +603,106 @@
   </sheetPr>
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O74" activeCellId="0" sqref="O74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="N2" s="0" t="n">
+      <c r="L2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -700,16 +710,16 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="A6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>281</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -723,10 +733,10 @@
       <c r="B7" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>284</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -797,7 +807,7 @@
       <c r="D11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1108,14 +1118,14 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,7 +1135,7 @@
       <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1136,7 +1146,7 @@
       <c r="B2" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">ROUND(B2/186, 3)</f>
         <v>0.043</v>
       </c>
@@ -1148,7 +1158,7 @@
       <c r="B3" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">ROUND(B3/186, 3)</f>
         <v>0.016</v>
       </c>
@@ -1160,7 +1170,7 @@
       <c r="B4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">ROUND(B4/186, 3)</f>
         <v>0.005</v>
       </c>
@@ -1172,7 +1182,7 @@
       <c r="B5" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">ROUND(B5/186, 3)</f>
         <v>0.081</v>
       </c>
@@ -1186,29 +1196,29 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>324</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>288</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>286</v>
       </c>
     </row>

</xml_diff>